<commit_message>
modified some errors needed to build qna part
</commit_message>
<xml_diff>
--- a/Preparation_test_0516/05_USECASE_식별자목록.xlsx
+++ b/Preparation_test_0516/05_USECASE_식별자목록.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>유스케이스 식별자 목록</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -253,6 +253,14 @@
   </si>
   <si>
     <t>구매하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>필수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -260,7 +268,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,21 +285,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="굴림"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="굴림"/>
       <family val="3"/>
       <charset val="129"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -308,12 +328,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,309 +624,372 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.125" customWidth="1"/>
-    <col min="2" max="2" width="18.125" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="3.5" customWidth="1"/>
-    <col min="5" max="5" width="12.125" customWidth="1"/>
-    <col min="6" max="6" width="18.125" customWidth="1"/>
-    <col min="7" max="7" width="17.5" customWidth="1"/>
-    <col min="8" max="8" width="3.5" customWidth="1"/>
-    <col min="9" max="9" width="12.125" customWidth="1"/>
-    <col min="10" max="10" width="18.125" customWidth="1"/>
-    <col min="11" max="11" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="12.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="I4" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="I7" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E8" t="s">
+      <c r="D8" s="4"/>
+      <c r="F8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
+      <c r="D9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E10" t="s">
+      <c r="D10" s="4"/>
+      <c r="F10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="I10" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="D11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="D12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="D13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="D14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="D15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="D16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="D17" s="4"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="F18" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="F19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H19" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="I19" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="C20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="F20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H20" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" t="s">
-        <v>39</v>
+      <c r="I20" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>